<commit_message>
Planejamento semanal em andamento e criação do mer básico
</commit_message>
<xml_diff>
--- a/Planejamentos/Planejamento semanal.xlsx
+++ b/Planejamentos/Planejamento semanal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Projeto_ProVagas\Planejamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C82E901-907F-4565-BFB5-35801AACD2E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E874B99-E6B2-4727-9B43-3A2E992C638B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
   <si>
     <t>PLANEJAMENTO SEMANAL - CONTROLE CLASSROOM</t>
   </si>
@@ -104,6 +104,42 @@
   </si>
   <si>
     <t>Alimentar o Azure</t>
+  </si>
+  <si>
+    <t>Modelo Físico</t>
+  </si>
+  <si>
+    <t>Normalização - Banco</t>
+  </si>
+  <si>
+    <t>Modelo Lógico</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Modelo Conceitual</t>
+  </si>
+  <si>
+    <t>DDL</t>
+  </si>
+  <si>
+    <t>DML</t>
+  </si>
+  <si>
+    <t>DQL</t>
+  </si>
+  <si>
+    <t>Planejamento BD</t>
+  </si>
+  <si>
+    <t>Mer - Modelo Entidade Relacionamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
@@ -179,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -259,11 +295,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -283,6 +330,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -299,7 +347,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,60 +568,60 @@
   </sheetPr>
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" customWidth="1"/>
     <col min="17" max="17" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="14"/>
     </row>
     <row r="2" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -588,64 +636,64 @@
       <c r="T2" s="3"/>
     </row>
     <row r="3" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14" t="s">
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="14" t="s">
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="14" t="s">
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="14"/>
     </row>
     <row r="4" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="15">
+      <c r="A4" s="16"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="16">
         <v>44020</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="15">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="16">
         <v>44021</v>
       </c>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="15">
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="16">
         <v>44022</v>
       </c>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="14"/>
     </row>
     <row r="5" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -710,110 +758,128 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="11" t="s">
         <v>24</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="N6" s="11" t="s">
         <v>24</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="19" t="s">
+      <c r="Q6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="R6" s="19" t="s">
+      <c r="R6" s="11" t="s">
         <v>24</v>
       </c>
       <c r="S6" s="6"/>
       <c r="T6" s="3"/>
     </row>
     <row r="7" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="6"/>
+      <c r="F7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="H7" s="3"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="I7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="K7" s="6"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="M7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="O7" s="6"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="Q7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="S7" s="6"/>
       <c r="T7" s="3"/>
     </row>
     <row r="8" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="7"/>
+      <c r="I8" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="J8" s="7"/>
       <c r="K8" s="6"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="6"/>
+      <c r="M8" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
       <c r="S8" s="6"/>
       <c r="T8" s="3"/>
     </row>
@@ -822,15 +888,23 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="G9" s="6"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="6"/>
+      <c r="I9" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="6"/>
+      <c r="M9" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="3"/>
@@ -844,16 +918,24 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="G10" s="6"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="6"/>
+      <c r="I10" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="M10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="11"/>
       <c r="O10" s="6"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="6"/>
@@ -866,16 +948,18 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="I11" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="11"/>
       <c r="K11" s="6"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
       <c r="O11" s="6"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="6"/>
@@ -888,13 +972,17 @@
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="11"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="I12" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="L12" s="3"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
@@ -910,7 +998,7 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -972,35 +1060,38 @@
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
     </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
     </row>
-    <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>20</v>
       </c>

</xml_diff>